<commit_message>
add multiple workFlow scripts
</commit_message>
<xml_diff>
--- a/inputFiles/eco_cost_inputs_GG_fixed.xlsx
+++ b/inputFiles/eco_cost_inputs_GG_fixed.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PhD\GitHubRepo\AWE-Eco\inputData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PhD\GitHubRepo\AWE-SE\inputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C61C26DC-9118-4F27-8C03-A665BB93A88E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1CB65FA-31D5-4DCF-BF68-13CCE746A51E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -730,7 +730,7 @@
   <dimension ref="A1:B33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update test coupling script to use YAML as input file for AWe-Power.
</commit_message>
<xml_diff>
--- a/inputFiles/eco_cost_inputs_GG_fixed.xlsx
+++ b/inputFiles/eco_cost_inputs_GG_fixed.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PhD\GitHubRepo\AWE-SE\inputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CC9F8D8-8B55-44BE-A501-DA881DD5324A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2405D3E4-F721-4B27-9AA2-E78E339AECDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="kite" sheetId="3" r:id="rId1"/>
@@ -545,13 +545,13 @@
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="29.140625" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="1" max="1" width="29.1796875" customWidth="1"/>
+    <col min="2" max="2" width="17.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -559,7 +559,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -567,7 +567,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -575,7 +575,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -583,7 +583,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -591,7 +591,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -599,7 +599,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>55</v>
       </c>
@@ -607,7 +607,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>51</v>
       </c>
@@ -615,7 +615,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>52</v>
       </c>
@@ -623,7 +623,7 @@
         <v>150000</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B13" s="1"/>
     </row>
   </sheetData>
@@ -639,13 +639,13 @@
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="27.85546875" customWidth="1"/>
-    <col min="2" max="2" width="23.42578125" customWidth="1"/>
+    <col min="1" max="1" width="27.81640625" customWidth="1"/>
+    <col min="2" max="2" width="23.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>25</v>
       </c>
@@ -654,7 +654,7 @@
       </c>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -663,7 +663,7 @@
       </c>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -671,7 +671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -679,7 +679,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -687,7 +687,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>48</v>
       </c>
@@ -695,7 +695,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>49</v>
       </c>
@@ -703,7 +703,7 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>50</v>
       </c>
@@ -711,7 +711,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>56</v>
       </c>
@@ -729,17 +729,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5144ACA-6792-40EA-A07E-EF86968317B7}">
   <dimension ref="A1:B33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.5703125" customWidth="1"/>
+    <col min="1" max="1" width="24.54296875" customWidth="1"/>
     <col min="2" max="2" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -747,7 +747,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -755,7 +755,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -763,7 +763,7 @@
         <v>2700</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -772,7 +772,7 @@
         <v>300000000</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -780,7 +780,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -788,7 +788,7 @@
         <v>7850</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -797,7 +797,7 @@
         <v>500000000</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>43</v>
       </c>
@@ -805,7 +805,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>44</v>
       </c>
@@ -813,7 +813,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -821,7 +821,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -829,7 +829,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -837,7 +837,7 @@
         <v>12.9</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -845,7 +845,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>29</v>
       </c>
@@ -853,7 +853,7 @@
         <v>0.71</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -861,7 +861,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -869,7 +869,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>31</v>
       </c>
@@ -877,7 +877,7 @@
         <v>12.4</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>33</v>
       </c>
@@ -885,7 +885,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>32</v>
       </c>
@@ -893,7 +893,7 @@
         <v>3400</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>57</v>
       </c>
@@ -901,7 +901,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>34</v>
       </c>
@@ -909,7 +909,7 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>35</v>
       </c>
@@ -918,7 +918,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>58</v>
       </c>
@@ -926,7 +926,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>59</v>
       </c>
@@ -935,7 +935,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>36</v>
       </c>
@@ -943,7 +943,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>37</v>
       </c>
@@ -951,7 +951,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>38</v>
       </c>
@@ -959,7 +959,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>39</v>
       </c>
@@ -967,7 +967,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>40</v>
       </c>
@@ -975,7 +975,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>41</v>
       </c>
@@ -983,7 +983,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>42</v>
       </c>
@@ -991,7 +991,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>53</v>
       </c>
@@ -999,7 +999,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>54</v>
       </c>
@@ -1021,12 +1021,12 @@
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" customWidth="1"/>
+    <col min="1" max="1" width="17.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -1034,7 +1034,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -1042,7 +1042,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -1050,7 +1050,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -1058,7 +1058,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -1079,7 +1079,7 @@
       <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1089,16 +1089,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{149E8716-C12E-4C74-BB23-8FB9587F4C00}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="27.28515625" customWidth="1"/>
+    <col min="1" max="1" width="27.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>45</v>
       </c>
@@ -1106,7 +1106,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>46</v>
       </c>
@@ -1114,7 +1114,7 @@
         <v>-1.2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>47</v>
       </c>

</xml_diff>

<commit_message>
Correct wing area and AR variation function. Update design space exploration scripts.
</commit_message>
<xml_diff>
--- a/inputFiles/eco_cost_inputs_GG_fixed.xlsx
+++ b/inputFiles/eco_cost_inputs_GG_fixed.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PhD\GitHubRepo\AWE-SE\inputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2405D3E4-F721-4B27-9AA2-E78E339AECDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{425B281F-91F1-4B23-9BCB-B1261B63C085}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="kite" sheetId="3" r:id="rId1"/>
@@ -729,7 +729,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5144ACA-6792-40EA-A07E-EF86968317B7}">
   <dimension ref="A1:B33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
@@ -923,7 +923,7 @@
         <v>58</v>
       </c>
       <c r="B23" s="1">
-        <v>180</v>
+        <v>400</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>